<commit_message>
feat: new settings generation
</commit_message>
<xml_diff>
--- a/[source]/generate/_generator/microbase.xlsx
+++ b/[source]/generate/_generator/microbase.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,36 +464,59 @@
           <t>replic-settings</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>replic-includes</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>replic-run</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>68</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve">&lt;!--
-npc="
-name:Грабитель:name
-ncolor:c0c0c0
-nattrib:-b
-fcolor:aaaaaa
-"
-hero="
-name:Я:name
-ncolor:ffffff
-nattrib:-b-n
-fattrib:-n
-fcolor:dddddd
-"
+	actors="hero; npc;"
+	&lt;actor.hero&gt;
+		name="Я"
+		&lt;default_active&gt;
+		&lt;wrap.act&gt;
+			!@ внешний вид кнопок для ответов.
+			$result += &lt;div class="avs-act-button"&gt;&lt;&lt;$args[2]&gt;&gt;&lt;/div&gt;
+		&lt;/wrap.act&gt;
+		&lt;wrap.frase&gt;
+			!@ внешний вид реплик в логе диалога Извлекаем имя из роли:
+			local $name_ = @em.tag.getNum(@edb.cell.getValue($args[0], 'sets', 'dialogs'), 'name')
+			$result += '&lt;div class="avs-hero-replic"&gt;'
+				$result += '&lt;span style="color:#ffffff;font-weight:bold;"&gt;&lt;&lt;$name_&gt;&gt;:&lt;/span&gt;'
+				$result += '&lt;span style="color:#dddddd;"&gt; — &lt;&lt;$args[2]&gt;&gt;:&lt;/span&gt;'
+			$result += '&lt;/div&gt;'
+		&lt;/wrap.frase&gt;
+	&lt;/actor.hero&gt;
+	&lt;actor.npc&gt;
+		name="Грабитель"
+		Здесь можно писать любой текст, он никак не повлияет на работу интерпретатора.
+		Обёртка для внешнего вида действий отсутствует, потому что данный персонаж общается только через пассивные реплики.
+		&lt;default_passive&gt;
+		&lt;wrap.frase&gt;
+			!@ внешний вид реплик в логе диалога Извлекаем имя из роли:
+			local $name_ = @em.tag.getNum(@edb.cell.getValue($args[0], 'sets', 'dialogs'), 'name')
+			$result += '&lt;div class="avs-hero-replic"&gt;'
+				$result += '&lt;span style="color:#c0c0c0;font-weight:bold;"&gt;&lt;&lt;$name_&gt;&gt;:&lt;/span&gt;'
+				$result += '&lt;span style="color:#aaaaaa;"&gt; — &lt;&lt;$args[2]&gt;&gt;:&lt;/span&gt;'
+			$result += '&lt;/div&gt;'
+		&lt;/wrap.frase&gt;
+	&lt;/actor.npc&gt;
+	strings:10
 --&gt;
-frase-block:
-&lt;npc-name&gt;У тебя одна минута на то, чтобы объяснить мне, как добраться до хранилища.
-&lt;hero-name&gt;Что?
-&lt;i&gt;Бац! В глазах сверкнуло и боль такая сильная, что кажется, будто она — единственное, что я сейчас чувствую. Даже сильнее страха.&lt;/i&gt;
-&lt;npc-name&gt;Одна минута, — &lt;i&gt;&lt;font color=#888888&gt;говорит он и прижимает холодный кружок дула к моему лбу.&lt;/font&gt;&lt;/i&gt;
-:frase-block
 </t>
         </is>
       </c>
@@ -514,25 +537,37 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-	marker:storagecellar
-	act-name:Хранилище в подвале...:act-name
-	Хранилище находится в подвале...
+repeat:cicle
+shuffle:straight
+act_length:25
+&lt;frase_block&gt;
+	&lt;actor:npc&gt;У тебя одна минута на то, чтобы объяснить мне, как добраться до хранилища.
+	&lt;actor:hero&gt;Что?
+	&lt;em&gt;Бац! В глазах сверкнуло и боль такая сильная, что кажется, будто она — единственное, что я сейчас чувствую. Даже сильнее страха.&lt;/em&gt;
+	&lt;actor:npc&gt;Одна минута, — &lt;em style="color:#888888;"&gt;говорит он и прижимает холодный кружок дула к моему лбу.&lt;/em&gt;
+&lt;/frase_block&gt;
 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>answer66</t>
+          <t>quest67</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -543,33 +578,40 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>66</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-	act-name:Но я здесь не работаю...:act-name
-	Но я здесь не работаю, я вообще не знаю, где тут что!
-</t>
+		marker:storagecellar
+		act-name:Хранилище в подвале...:act-name
+		Хранилище находится в подвале...
+	</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>answer19</t>
+          <t>answer66</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>quest67</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -579,27 +621,35 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Что?
-</t>
+          <t xml:space="preserve">
+		act-name:Но я здесь не работаю...:act-name
+		Но я здесь не работаю, я вообще не знаю, где тут что!
+	</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>answer4</t>
+          <t>answer19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>quest67</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -609,63 +659,69 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-		marker:thirddead
-		iffing:DIALOG_VALUE["что.в"]=1:iffing
-		npc="name::name tire:nope fattrib:-i"
-		Он стискивает зубы и стреля...
-		dynamic-code:cla:dynamic-code
+          <t xml:space="preserve">Что?
 	</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>quest3</t>
+          <t>answer4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>answer4</t>
+          <t>quest67</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-		iffing:DIALOG_VALUE["что.в"]=0:iffing
-		dynamic-code:DIALOG_VALUE["что.в"]=1:dynamic-code
-		frase-block:
-			&lt;i&gt;Бац! Оказывается, может быть ещё больнее, чем в первый раз.&lt;/i&gt;
-			&lt;npc-name&gt;Ещё раз скажешь «что», выстрелю.
-		:frase-block
-	</t>
+			marker:thirddead
+			&lt;if&gt;DIALOG_VALUE["что.в"]=1&lt;/if&gt;
+			npc="name::name tire:nope fattrib:-i"
+			Он стискивает зубы и стреля...
+			&lt;dynamic_code&gt;cla&lt;/dynamic_code&gt;
+		</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>quest1</t>
+          <t>quest3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -680,118 +736,143 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[Закрыть]closeup</t>
+          <t xml:space="preserve">
+			&lt;if&gt;DIALOG_VALUE["что.в"]=0&lt;/if&gt;
+			&lt;dynamic_code&gt;DIALOG_VALUE["что.в"]=1&lt;/dynamic_code&gt;
+			&lt;frase_block&gt;
+				&lt;em&gt;Бац! Оказывается, может быть ещё больнее, чем в первый раз.&lt;/em&gt;
+				&lt;actor:npc&gt;Ещё раз скажешь «что», выстрелю.
+			&lt;/frase_block&gt;
+		</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>answer2</t>
+          <t>quest1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>quest3</t>
+          <t>answer4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Какого чёрта тогда ты делаешь в кабинке оператора?
-	</t>
+          <t>[Закрыть]closeup</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>answer2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>answer19</t>
+          <t>quest3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-			act-name:Тоже решил денег взять.:act-name
-			Да я вот решил тоже денег взять. Под шумок, так сказать. Хе-хе.
+          <t xml:space="preserve">Какого чёрта тогда ты делаешь в кабинке оператора?
 		</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>answer17</t>
+          <t>quest18</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>answer19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			От вас прячусь.
-			frase-block:
-				&lt;hero-name&gt;Я тут от вас прячусь...
-				&lt;npc-name&gt;А, ты один из посетителей?
-				&lt;hero-name&gt;Да.
-				&lt;npc-name&gt;Я вот не видел, ка</t>
+				act-name:Тоже решил денег взять.:act-name
+				Да я вот решил тоже денег взять. Под шумок, так сказать. Хе-хе.
+			</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>answer14</t>
+          <t>answer17</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -806,24 +887,37 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			act-name:Я техник.:act-name
-			Я просто техник, мне позвонили и попросили починить компьютер. Они иногда вызывают меня сюда, но я не знаю, где тут сейф, честное слово!
-		</t>
+				От вас прячусь.
+				&lt;frase_block&gt;
+					&lt;actor:hero&gt;Я тут от вас прячусь...
+					&lt;actor:npc&gt;А, ты один из посетителей?
+					&lt;actor:hero&gt;Да.
+					&lt;actor:npc&gt;Я вот не видел, как ты сюда пробегал, ты сюда зашёл ещё до того, как я вошёл в здание?
+					&lt;actor:hero&gt;Да!
+					&lt;actor:npc&gt;А как же ты через турникет прошёл?
+				&lt;/frase_block&gt;
+			</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>answer10</t>
+          <t>answer14</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -838,88 +932,104 @@
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-				Занятно. Тогда почему на твоём бейдже написано «Старший кассир»?
+				act-name:Я техник.:act-name
+				Я просто техник, мне позвонили и попросили починить компьютер. Они иногда вызывают меня сюда, но я не знаю, где тут сейф, честное слово!
 			</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>quest9</t>
+          <t>answer10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>answer10</t>
+          <t>quest18</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-					act-name:Хранилище в подвале...:act-name
-					leveljump:storagecellar
-				</t>
+					Занятно. Тогда почему на твоём б</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>answer8</t>
+          <t>quest9</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>quest9</t>
+          <t>answer10</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-					hero="nattrib:-i"
-					act-name:Я его одолжил, чтобы через турникет пройти.:act-name
-					Я его одолжил, чтобы пройти через турникет, я часто так делаю, а то они никак мне собственный не сделают...
-				</t>
+						act-name:Хранилище в подвале...:act-name
+						leveljump:storagecellar
+					</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>answer7</t>
+          <t>answer8</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -934,150 +1044,182 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-						frase-block:
-						&lt;npc-name&gt;У кого одолжил?
-						&lt;i&gt;Пальцем в толстого очкарика на полу, тут же затрясшего головой.&lt;/i&gt;
-						&lt;npc-name&gt;Окей, спасибо, техник, — &lt;i&gt;и спускает куро...&lt;i&gt;
-						:frase-block
-						dynamic-code:cla:dynamic-code
+						hero="nattrib:-i"
+						act-name:Я его одолжил, чтобы через турникет пройти.:act-name
+						Я его одолжил, чтобы пройти через турникет, я часто так делаю, а то они никак мне собственный не сделают...
 					</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>quest6</t>
+          <t>answer7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>answer7</t>
+          <t>quest9</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[Закрыть]closeup</t>
+          <t xml:space="preserve">
+							&lt;frase_block&gt;
+							&lt;actor:npc&gt;У кого одолжил?
+							&lt;em&gt;Пальцем в толстого очкарика на полу, тут же затрясшего головой.&lt;/em&gt;
+							&lt;actor:npc&gt;Окей, спасибо, техник, — &lt;i&gt;и спускает куро...&lt;i&gt;
+							&lt;/frase_block&gt;
+							&lt;dynamic_code&gt;cla&lt;/dynamic_code&gt;
+						</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>answer5</t>
+          <t>quest6</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>quest6</t>
+          <t>answer7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-			</t>
+          <t>[Закрыть]closeup</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>quest13</t>
+          <t>answer5</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>answer14</t>
+          <t>quest6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
           <t xml:space="preserve">
-					act-name:Хранилище в подвале...:act-name
-					leveljump:storagecellar
 				</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>answer12</t>
+          <t>quest13</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>quest13</t>
+          <t>answer14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Что?
-					leveljump:thirddead
-				</t>
+          <t xml:space="preserve">
+						act-name:Хранилище в подвале...:act-name
+						leveljump:storagecellar
+					</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>answer11</t>
+          <t>answer12</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1092,119 +1234,144 @@
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">А, вон оно что. Но на тебе форма сотрудника банка. То есть, ты не только лжец, но ещё и вор? Двадцать секунд. Хе-хе.
-			</t>
+          <t xml:space="preserve">Что?
+						leveljump:thirddead
+					</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>quest16</t>
+          <t>answer11</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>answer17</t>
+          <t>quest13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-					act-name:Хранилище в подвале!:act-name
-					leveljump:storagecellar
+          <t xml:space="preserve">А, вон оно что. Но на тебе форма сотрудника банка. То есть, ты не только лжец, но ещё и вор? Двадцать секунд. Хе-хе.
 				</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>answer15</t>
+          <t>quest16</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>quest16</t>
+          <t>answer17</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Уже лучше. А теперь, как туда добраться?
-	</t>
+          <t xml:space="preserve">
+						act-name:Хранилище в подвале!:act-name
+						leveljump:storagecellar
+					</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>quest65</t>
+          <t>answer15</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>answer66</t>
+          <t>quest16</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-	</t>
+          <t xml:space="preserve">Уже лучше. А теперь, как туда добраться?
+		</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>quest65</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>quest65</t>
+          <t>answer66</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1214,56 +1381,66 @@
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Нет:act-name
-			iffing:$DIALOG_VALUE["по лестнице"]="поговорили" and $DIALOG_VALUE["по лифту"]="поговорили":iffing
-			К сожалению, больше путей нет.
+          <t xml:space="preserve">
 		</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>answer63</t>
+          <t>quest64</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>quest65</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:На лифте...:act-name
-			iffing:$DIALOG_VALUE["по лифту"]!"поговорили":iffing
-			В кабинете управляющего есть лифт, спускающийся прямо в хранилище. Только вряд ли вы до него доберётесь.
-		</t>
+          <t xml:space="preserve">act-name:Нет:act-name
+				&lt;if&gt;$DIALOG_VALUE["по лестнице"]="поговорили" and $DIALOG_VALUE["по лифту"]="поговорили"&lt;/if&gt;
+				К сожалению, больше путей нет.
+			</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>answer58</t>
+          <t>answer63</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1278,24 +1455,30 @@
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:По лестнице...:act-name
-			iffing:$DIALOG_VALUE["по лестнице"]!"поговорили":iffing
-			Вон за той дверью в подвал ведёт лестница, по ней можно спуститься до главного коридора, из него в архив, а уже через архив к двери хранилища.
-		</t>
+          <t xml:space="preserve">act-name:На лифте...:act-name
+				&lt;if&gt;$DIALOG_VALUE["по лифту"]!"поговорили"&lt;/if&gt;
+				В кабинете управляющего есть лифт, спускающийся прямо в хранилище. Только вряд ли вы до него доберётесь.
+			</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>answer39</t>
+          <t>answer58</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1310,57 +1493,71 @@
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ещё что-нибудь, о чём мне как грабителю полезно было бы узнать?
+          <t xml:space="preserve">act-name:По лестнице...:act-name
+				&lt;if&gt;$DIALOG_VALUE["по лестнице"]!"поговорили"&lt;/if&gt;
+				Вон за той дверью в подвал ведёт лестница, по ней можно спуститься до главного коридора, из него в архив, а уже через архив к двери хранилища.
 			</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>quest38</t>
+          <t>answer39</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>answer39</t>
+          <t>quest64</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Ещё что-нибудь, о чём мне как грабителю полезно было бы узнать?
 				</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>quest38</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>quest38</t>
+          <t>answer39</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1370,34 +1567,33 @@
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-						iffing:$DIALOG_VALUE["хранилище"]="поговорили" and $DIALOG_VALUE["архив"]="поговорили" and $DIALOG_VALUE["коридор"]="поговорили" and $DIALOG_VALUE["лестница"]="поговорили":iffing
-						dynamic-code:$DIALOG_VALUE["по лестнице"]="поговорили":dynamic-code
-						frase-block:
-						&lt;hero-name&gt;На этом всё.
-						&lt;npc-name&gt;А другой путь есть?
-						:frase-block
-						levelup:4
 					</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>quest36</t>
+          <t>quest37</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>quest38</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1407,24 +1603,35 @@
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:О двери в хранилище...:act-name
-						Толщина двери в хранилище полтора метра.
-						iffing:$DIALOG_VALUE["хранилище"]!"поговорили":iffing
-					</t>
+          <t xml:space="preserve">
+							&lt;if&gt;$DIALOG_VALUE["хранилище"]="поговорили" and $DIALOG_VALUE["архив"]="поговорили" and $DIALOG_VALUE["коридор"]="поговорили" and $DIALOG_VALUE["лестница"]="поговорили"&lt;/if&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["по лестнице"]="поговорили"&lt;/dynamic_code&gt;
+							&lt;frase_block&gt;
+							&lt;actor:hero&gt;На этом всё.
+							&lt;actor:npc&gt;А другой путь есть?
+							&lt;/frase_block&gt;
+							levelup:4
+						</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>answer35</t>
+          <t>quest36</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1435,28 +1642,34 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Об архиве...:act-name
-						iffing:$DIALOG_VALUE["архив"]!"поговорили":iffing
-						В архиве люди пропадают...
-					</t>
+          <t xml:space="preserve">act-name:О двери в хранилище...:act-name
+							Толщина двери в хранилище полтора метра.
+							&lt;if&gt;$DIALOG_VALUE["хранилище"]!"поговорили"&lt;/if&gt;
+						</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>answer33</t>
+          <t>answer35</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1471,24 +1684,28 @@
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:О коридоре...:act-name
-						iffing:$DIALOG_VALUE["коридор"]!"поговорили":iffing
-						Поперёк коридора идут лазерные лучи.
-					</t>
+          <t xml:space="preserve">act-name:Об архиве...:act-name
+							&lt;if&gt;$DIALOG_VALUE["архив"]!"по</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>answer31</t>
+          <t>answer33</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1503,24 +1720,30 @@
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:О лестинце...:act-name
-						iffing:$DIALOG_VALUE["лестница"]!"поговорили":iffing
-						На лестнице сторожит охранник с оружием.
-					</t>
+          <t xml:space="preserve">act-name:О коридоре...:act-name
+							&lt;if&gt;$DIALOG_VALUE["коридор"]!"поговорили"&lt;/if&gt;
+							Поперёк коридора идут лазерные лучи.
+						</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>answer25</t>
+          <t>answer31</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1535,84 +1758,103 @@
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Каким оружием?
+          <t xml:space="preserve">act-name:О лестинце...:act-name
+							&lt;if&gt;$DIALOG_VALUE["лестница"]!"поговорили"&lt;/if&gt;
+							На лестнице сторожит охранник с оружием.
 						</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>quest24</t>
+          <t>answer25</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>answer25</t>
+          <t>quest37</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Benelli M4...:act-name
-								Benelli M4 Super 90, шестизарядный, с телескопическим прикладом, пистолетной рукояткой, планкой Пикатинни...
+          <t xml:space="preserve">Каким оружием?
 							</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>answer23</t>
+          <t>quest24</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>quest24</t>
+          <t>answer25</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Ружьё какое-то...:act-name
-								Не знаю, я не разбираюсь.
-							</t>
+          <t xml:space="preserve">act-name:Benelli M4...:act-name
+									Benelli M4 Super 90, шестизарядный, с телескопическим прикладом, пистолетной рукояткой, планкой Пикатинни...
+								</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>answer21</t>
+          <t>answer23</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1627,61 +1869,72 @@
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Дальше.
-									dynamic-code:$DIALOG_VALUE["лестница"]="поговорили":dynamic-code
-									levelup:4
+          <t xml:space="preserve">act-name:Ружьё какое-то...:act-name
+									Не знаю, я не разбираюсь.
 								</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>quest20</t>
+          <t>answer21</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>answer21</t>
+          <t>quest24</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Всё, заткнись, давай дальше.
-									dynamic-code:$DIALOG_VALUE["лестница"]="поговорили":dynamic-code
-									levelup:4
-								</t>
+          <t xml:space="preserve">Дальше.
+										&lt;dynamic_code&gt;$DIALOG_VALUE["лестница"]="поговорили"&lt;/dynamic_code&gt;
+										levelup:4
+									</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>quest22</t>
+          <t>quest20</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>answer23</t>
+          <t>answer21</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1691,27 +1944,35 @@
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Красные или зелёные?
-						</t>
+          <t xml:space="preserve">Всё, заткнись, давай дальше.
+										&lt;dynamic_code&gt;$DIALOG_VALUE["лестница"]="поговорили"&lt;/dynamic_code&gt;
+										levelup:4
+									</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>quest30</t>
+          <t>quest22</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>answer31</t>
+          <t>answer23</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1721,62 +1982,73 @@
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Зелёные.:act-name
-								dynamic-code:cla:dynamic-code
-								frase-block:
-									&lt;hero-name&gt;Зелёные, кажется, а что?
-									&lt;npc-name&gt;Проклятье, у меня дейтеранопия.
-									&lt;hero-name&gt;Зелёный цвет не различаете?
-									&lt;npc-name&gt;Да.
-									&lt;hero-name&gt;Сочувствую.
-									&lt;npc-name&gt;Спасибо. Дальше.
-								:frase-block
+          <t xml:space="preserve">Красные или зелёные?
 							</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>answer29</t>
+          <t>quest30</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>quest30</t>
+          <t>answer31</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Красные.:act-name
-								Красные, кажется. А что есть какая-то разница?
-							</t>
+          <t xml:space="preserve">act-name:Зелёные.:act-name
+									&lt;dynamic_code&gt;cla&lt;/dynamic_code&gt;
+									&lt;frase_block&gt;
+										&lt;actor:hero&gt;Зелёные, кажется, а что?
+										&lt;actor:npc&gt;Проклятье, у меня дейтеранопия.
+										&lt;actor:hero&gt;Зелёный цвет не различаете?
+										&lt;actor:npc&gt;Да.
+										&lt;actor:hero&gt;Сочувствую.
+										&lt;actor:npc&gt;Спасибо. Дальше.
+									&lt;/frase_block&gt;
+								</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>answer27</t>
+          <t>answer29</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1791,61 +2063,72 @@
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Не твоего ума дело, дальше давай.
-									dynamic-code:$DIALOG_VALUE["коридор"]="поговорили":dynamic-code
-									levelup:4
+          <t xml:space="preserve">act-name:Красные.:act-name
+									Красные, кажется. А что есть какая-то разница?
 								</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>quest26</t>
+          <t>answer27</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>answer27</t>
+          <t>quest30</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-									dynamic-code:$DIALOG_VALUE["коридор"]="поговорили":dynamic-code
-									levelup:4
-								</t>
+          <t xml:space="preserve">Не твоего ума дело, дальше давай.
+										&lt;dynamic_code&gt;$DIALOG_VALUE["коридор"]="поговорили"&lt;/dynamic_code&gt;
+										levelup:4
+									</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>quest28</t>
+          <t>quest26</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>answer29</t>
+          <t>answer27</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1855,40 +2138,35 @@
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-						frase-block:
-							&lt;npc-name&gt;Что?!
-							&lt;hero-name&gt;Люди, говорю, в архиве пропадают.
-							&lt;npc-name&gt;Да это я понял! Почему пропадают?
-							&lt;hero-name&gt;Не знаю, но, поговаривают, что нужно быть поосторожнее со шкафами "Ф".
-							&lt;npc-name&gt;Почему?
-							&lt;hero-name&gt;Пропали сотрудники Фриманн, Фрекель, Фаркопс и Фонг. У вас какая фамилия?
-							&lt;npc-name&gt;Фицжеральд.
-							&lt;hero-name&gt;О...
-							&lt;npc-name&gt;Дальше.
-						:frase-block
-						dynamic-code:$DIALOG_VALUE["архив"]="поговорили":dynamic-code
-						levelup:2
-						</t>
+										&lt;dynamic_code&gt;$DIALOG_VALUE["коридор"]="поговорили"&lt;/dynamic_code&gt;
+										levelup:4
+									</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>quest32</t>
+          <t>quest28</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>answer33</t>
+          <t>answer29</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1898,38 +2176,46 @@
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-						frase-block:
-							&lt;npc-name&gt;Ого...
-							&lt;hero-name&gt;И замок «Sargent &amp; Greenleaf».
-							&lt;npc-name&gt;Ой...
-							&lt;hero-name&gt;Пол внутри под напряжением десять тысяч вольт.
-							&lt;npc-name&gt;Ох...
-							&lt;hero-name&gt;А снаружи камеры.
-							&lt;npc-name&gt;Понятно. Дальше.
-						:frase-block
-						dynamic-code:$DIALOG_VALUE["хранилище"]="поговорили":dynamic-code
-						levelup:2
-						</t>
+							&lt;frase_block&gt;
+								&lt;actor:npc&gt;Что?!
+								&lt;actor:hero&gt;Люди, говорю, в архиве пропадают.
+								&lt;actor:npc&gt;Да это я понял! Почему пропадают?
+								&lt;actor:hero&gt;Не знаю, но, поговаривают, что нужно быть поосторожнее со шкафами "Ф".
+								&lt;actor:npc&gt;Почему?
+								&lt;actor:hero&gt;Пропали сотрудники Фриманн, Фрекель, Фаркопс и Фонг. У вас какая фамилия?
+								&lt;actor:npc&gt;Фицжеральд.
+								&lt;actor:hero&gt;О...
+								&lt;actor:npc&gt;Дальше.
+							&lt;/frase_block&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["архив"]="поговорили"&lt;/dynamic_code&gt;
+							levelup:2
+							</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>quest34</t>
+          <t>quest32</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>answer35</t>
+          <t>answer33</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1939,28 +2225,44 @@
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
           <t xml:space="preserve">
-				Почему это?
-			</t>
+							&lt;frase_block&gt;
+								&lt;actor:npc&gt;Ого...
+								&lt;actor:hero&gt;И замок «Sargent &amp; Greenleaf».
+								&lt;actor:npc&gt;Ой...
+								&lt;actor:hero&gt;Пол внутри под напряжением десять тысяч вольт.
+								&lt;actor:npc&gt;Ох...
+								&lt;actor:hero&gt;А снаружи камеры.
+								&lt;actor:npc&gt;Понятно. Дальше.
+							&lt;/frase_block&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["хранилище"]="поговорили"&lt;/dynamic_code&gt;
+							levelup:2
+							</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>quest57</t>
+          <t>quest34</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>answer58</t>
+          <t>answer35</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1970,29 +2272,34 @@
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>57</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
           <t xml:space="preserve">
-				&lt;!-- блок действий --&gt;
-				&lt;!-- блок действий --&gt;
+					Почему это?
 				</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>quest57</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>quest57</t>
+          <t>answer58</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -2002,34 +2309,35 @@
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
           <t xml:space="preserve">
-						iffing:$DIALOG_VALUE["системы идентификации"]="поговорили" and $DIALOG_VALUE["собаки"]="поговорили" and $DIALOG_VALUE["управляющий"]="поговорили":iffing
-						dynamic-code:$DIALOG_VALUE["по лифту"]="поговорили":dynamic-code
-						frase-block:
-							&lt;hero-name&gt;Это всё.
-							&lt;npc-name&gt;А другой путь есть?
-						:frase-block
-						levelup:4
+					&lt;!-- блок действий --&gt;
+					&lt;!-- блок действий --&gt;
 					</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>quest55</t>
+          <t>quest56</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>quest57</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -2039,24 +2347,35 @@
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Системы идентификации.:act-name
-						iffing:$DIALOG_VALUE["системы идентификации"]!"поговорили":iffing
-						В лифте стоят системы идентификации, которые пропускают только управляющего.
-					</t>
+          <t xml:space="preserve">
+							&lt;if&gt;$DIALOG_VALUE["системы идентификации"]="поговорили" and $DIALOG_VALUE["собаки"]="поговорили" and $DIALOG_VALUE["управляющий"]="поговорили"&lt;/if&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["по лифту"]="поговорили"&lt;/dynamic_code&gt;
+							&lt;frase_block&gt;
+								&lt;actor:hero&gt;Это всё.
+								&lt;actor:npc&gt;А другой путь есть?
+							&lt;/frase_block&gt;
+							levelup:4
+						</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>answer54</t>
+          <t>quest55</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2067,27 +2386,34 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Собаки.
-						iffing:$DIALOG_VALUE["собаки"]!"поговорили":iffing
-					</t>
+          <t xml:space="preserve">act-name:Системы идентификации.:act-name
+							&lt;if&gt;$DIALOG_VALUE["системы идентификации"]!"поговорили"&lt;/if&gt;
+							В лифте стоят системы идентификации, которые пропускают только управляющего.
+						</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>answer43</t>
+          <t>answer54</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2102,24 +2428,29 @@
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Управляющий.:act-name
-						iffing:$DIALOG_VALUE["управляющий"]!"поговорили":iffing
-						В кабинете скорее всего сидит сам управляющий.
-					</t>
+          <t xml:space="preserve">Собаки.
+							&lt;if&gt;$DIALOG_VALUE["собаки"]!"поговорили"&lt;/if&gt;
+						</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>answer41</t>
+          <t>answer43</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2134,74 +2465,78 @@
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve">frase-block:&lt;npc-name&gt;И чего?
-							&lt;hero-name&gt;Он чемпион города по гарлемскому боксу.
-							&lt;npc-name&gt;Впервые слышу про такой бокс.
-							&lt;hero-name&gt;Основная особенность его в том, что во время боя разрешено использовать кастеты, биты и автоматическое оружие.
-							&lt;npc-name&gt;Хмм, ну ладно, допустим, я с ним разберусь, что ещё?
-						:frase-block
-						dynamic-code:$DIALOG_VALUE["управляющий"]="поговорили":dynamic-code
-						levelup:2
+          <t xml:space="preserve">act-name:Управляющий.:act-name
+							&lt;if&gt;$DIALOG_VALUE["управляющий"]!"поговорили"&lt;/if&gt;
+							В кабинете скорее всего сидит сам управляющий.
 						</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>quest40</t>
+          <t>answer41</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>answer41</t>
+          <t>quest56</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">frase-block:
-							&lt;npc-name&gt;Собаки?
-							&lt;hero-name&gt;Да.
-							&lt;npc-name&gt;Большие?
-							&lt;hero-name&gt;Очень.
-							&lt;npc-name&gt;Много?
-							&lt;hero-name&gt;Четыре.
-							&lt;npc-name&gt;Ох... Ну допустим, с собаками я как-нибудь управлюсь. Что-то ещё?
-						:frase-block
-						dynamic-code:$DIALOG_VALUE["собаки"]="поговорили":dynamic-code
-						levelup:2
-						</t>
+          <t xml:space="preserve">&lt;actor:frase_block&gt;&lt;npc&gt;И чего?
+								&lt;actor:hero&gt;Он чемпион города по гарлемскому боксу.
+								&lt;actor:npc&gt;Впервые слышу про такой бокс.
+								&lt;actor:hero&gt;Основная особенность его в том, что во время боя разрешено использовать кастеты, биты и автоматическое оружие.
+								&lt;actor:npc&gt;Хмм, ну ладно, допустим, я с ним разберусь, что ещё?
+							&lt;/frase_block&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["управляющий"]="поговорили"&lt;/dynamic_code&gt;
+							levelup:2
+							</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>quest42</t>
+          <t>quest40</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>answer43</t>
+          <t>answer41</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -2211,27 +2546,43 @@
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Какие системы?
-						</t>
+          <t xml:space="preserve">&lt;frase_block&gt;
+								&lt;actor:npc&gt;Собаки?
+								&lt;actor:hero&gt;Да.
+								&lt;actor:npc&gt;Большие?
+								&lt;actor:hero&gt;Очень.
+								&lt;actor:npc&gt;Много?
+								&lt;actor:hero&gt;Четыре.
+								&lt;actor:npc&gt;Ох... Ну допустим, с собаками я как-нибудь управлюсь. Что-то ещё?
+							&lt;/frase_block&gt;
+							&lt;dynamic_code&gt;$DIALOG_VALUE["собаки"]="поговорили"&lt;/dynamic_code&gt;
+							levelup:2
+							</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>quest53</t>
+          <t>quest42</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>answer54</t>
+          <t>answer43</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -2241,29 +2592,33 @@
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-							&lt;!-- системы идентификации --&gt;
-							&lt;!-- системы идентификации --&gt;
+          <t xml:space="preserve">Какие системы?
 							</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>quest53</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>quest53</t>
+          <t>answer54</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -2273,56 +2628,68 @@
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:По системам всё:act-name
-									По системам идентификации всё.
-									iffing:$DIALOG_VALUE["вес"]="поговорили" and $DIALOG_VALUE["сетчатка"]="поговорили" and $DIALOG_VALUE["отпечатки"]="поговорили":iffing
+          <t xml:space="preserve">
+								&lt;!-- системы идентификации --&gt;
+								&lt;!-- системы идентификации --&gt;
 								</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>answer51</t>
+          <t>quest52</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>quest53</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Вес:act-name
-									Датчик веса.
-									iffing:$DIALOG_VALUE["вес"]!"поговорили":iffing
-								</t>
+          <t xml:space="preserve">act-name:По системам всё:act-name
+										По системам идентификации всё.
+										&lt;if&gt;$DIALOG_VALUE["вес"]="поговорили" and $DIALOG_VALUE["сетчатка"]="поговорили" and $DIALOG_VALUE["отпечатки"]="поговорили"&lt;/if&gt;
+									</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>answer49</t>
+          <t>answer51</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2337,24 +2704,30 @@
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Сетчатка глаза.:act-name
-									Сканер сетчатки глаза.
-									iffing:$DIALOG_VALUE["сетчатка"]!"поговорили":iffing
-								</t>
+          <t xml:space="preserve">act-name:Вес:act-name
+										Датчик веса.
+										&lt;if&gt;$DIALOG_VALUE["вес"]!"поговорили"&lt;/if&gt;
+									</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>answer47</t>
+          <t>answer49</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2369,24 +2742,30 @@
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Отпечатки.:act-name
-									Сканер отпечатка правой ладони.
-									iffing:$DIALOG_VALUE["отпечатки"]!"поговорили":iffing
-								</t>
+          <t xml:space="preserve">act-name:Сетчатка глаза.:act-name
+										Сканер сетчатки глаза.
+										&lt;if&gt;$DIALOG_VALUE["сетчатка"]!"поговорили"&lt;/if&gt;
+									</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>answer45</t>
+          <t>answer47</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2401,61 +2780,73 @@
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Это, теоретически, можно обойти. Дальше.
-										dynamic-code:$DIALOG_VALUE["отпечатки"]="поговорили":dynamic-code
-										levelup:2
+          <t xml:space="preserve">act-name:Отпечатки.:act-name
+										Сканер отпечатка правой ладони.
+										&lt;if&gt;$DIALOG_VALUE["отпечатки"]!"поговорили"&lt;/if&gt;
 									</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>quest44</t>
+          <t>answer45</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>answer45</t>
+          <t>quest52</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Для этого у меня есть инструменты и необходимые навыки, — &lt;i&gt;он зловеще ухмыляется.&lt;/i&gt; — Дальше.
-										dynamic-code:$DIALOG_VALUE["сетчатка"]="поговорили":dynamic-code
-										levelup:2
-									</t>
+          <t xml:space="preserve">Это, теоретически, можно обойти. Дальше.
+											&lt;dynamic_code&gt;$DIALOG_VALUE["отпечатки"]="поговорили"&lt;/dynamic_code&gt;
+											levelup:2
+										</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>quest46</t>
+          <t>quest44</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>answer47</t>
+          <t>answer45</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -2465,34 +2856,35 @@
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-									frase-block:
-										&lt;npc-name&gt;Хм. Сколько весит местный управляющий?
-										&lt;hero-name&gt;124 килограмма. А вы сколько весите?
-										&lt;npc-name&gt;61. Мда. Тут даже клонирующая машина бы не помогла. Ладно, дальше.
-									:frase-block
-									dynamic-code:$DIALOG_VALUE["вес"]="поговорили":dynamic-code
-									levelup:2
-									</t>
+          <t xml:space="preserve">Для этого у меня есть инструменты и необходимые навыки, — &lt;em&gt;он зловеще ухмыляется.&lt;/em&gt; — Дальше.
+											&lt;dynamic_code&gt;$DIALOG_VALUE["сетчатка"]="поговорили"&lt;/dynamic_code&gt;
+											levelup:2
+										</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>quest48</t>
+          <t>quest46</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>answer49</t>
+          <t>answer47</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -2502,29 +2894,40 @@
         </is>
       </c>
       <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ещё что-нибудь по лифту?
-										dynamic-code:$DIALOG_VALUE["системы идентификации"]="поговорили":dynamic-code
-										levelup:5
-									</t>
+          <t xml:space="preserve">
+										&lt;frase_block&gt;
+											&lt;actor:npc&gt;Хм. Сколько весит местный управляющий?
+											&lt;actor:hero&gt;124 килограмма. А вы сколько весите?
+											&lt;actor:npc&gt;61. Мда. Тут даже клонирующая машина бы не помогла. Ладно, дальше.
+										&lt;/frase_block&gt;
+										&lt;dynamic_code&gt;$DIALOG_VALUE["вес"]="поговорили"&lt;/dynamic_code&gt;
+										levelup:2
+										</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>quest50</t>
+          <t>quest48</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>answer51</t>
+          <t>answer49</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -2534,28 +2937,35 @@
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-				Вот же задачка. Монетку бросить что ли... Это всё? Может ещё что-нибудь знаешь?
-			</t>
+          <t xml:space="preserve">Ещё что-нибудь по лифту?
+											&lt;dynamic_code&gt;$DIALOG_VALUE["системы идентификации"]="поговорили"&lt;/dynamic_code&gt;
+											levelup:5
+										</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>quest62</t>
+          <t>quest50</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>answer63</t>
+          <t>answer51</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -2565,106 +2975,167 @@
         </is>
       </c>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t xml:space="preserve">act-name:Про деньги.:act-name
-					Знаю про деньги в хранилище.
+          <t xml:space="preserve">
+					Вот же задачка. Монетку бросить что ли... Это всё? Может ещё что-нибудь знаешь?
 				</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>answer61</t>
+          <t>quest62</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>quest62</t>
+          <t>answer63</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-					frase-block:
-						&lt;npc-name&gt;Так, и что с ними?
-						&lt;hero-name&gt;Их там нет.
-						&lt;npc-name&gt;Как нет?!
-						&lt;hero-name&gt;Ну мы переезжаем в другой район города и все деньги и ценности уже перевезли сегодня ночью.
-						&lt;npc-name&gt;Так почему ты сразу не сказал?!
-						&lt;hero-name&gt;Ну про это вы как раз не спрашивали.
-						&lt;npc-name&gt;Проклятье!
-						&lt;i&gt;И с этими словами он выбегает из отделения банка, где его ловит экипаж инкассаторской машины, приехавшей, чтобы как раз перевезти содержимое хранилища в другой район города. Хе-хе.&lt;/i&gt;
-					:frase-block
+          <t xml:space="preserve">act-name:Про деньги.:act-name
+						Знаю про деньги в хранилище.
 					</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>quest60</t>
+          <t>answer61</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>answer61</t>
+          <t>quest62</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>answer</t>
         </is>
       </c>
       <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[Закрыть]closeup</t>
+          <t xml:space="preserve">
+						&lt;frase_block&gt;
+							&lt;actor:npc&gt;Так, и что с ними?
+							&lt;actor:hero&gt;Их там нет.
+							&lt;actor:npc&gt;Как нет?!
+							&lt;actor:hero&gt;Ну мы переезжаем в другой район города и все деньги и ценности уже перевезли сегодня ночью.
+							&lt;actor:npc&gt;Так почему ты сразу не сказал?!
+							&lt;actor:hero&gt;Ну про это вы как раз не спрашивали.
+							&lt;actor:npc&gt;Проклятье!
+							&lt;em&gt;И с этими словами он выбегает из отделения банка, где его ловит экипаж инкассаторской машины, приехавшей, чтобы как раз перевезти содержимое хранилища в другой район города. Хе-хе.&lt;/em&gt;
+						&lt;/frase_block&gt;
+						</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>answer59</t>
+          <t>quest60</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>quest60</t>
+          <t>answer61</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>answer</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>[Закрыть]closeup</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>answer59</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>quest60</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>answer</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>